<commit_message>
Add data entry html file; correct html errors
</commit_message>
<xml_diff>
--- a/ExcelCo/basics/02_data_entry.xlsx
+++ b/ExcelCo/basics/02_data_entry.xlsx
@@ -459,16 +459,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -481,9 +484,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -986,8 +986,8 @@
       <c r="K4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
       <c r="N4" s="9"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
@@ -1003,8 +1003,8 @@
       <c r="K5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
       <c r="N5" s="9"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
@@ -1020,8 +1020,8 @@
       <c r="K6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
       <c r="N6" s="9"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
@@ -1037,8 +1037,8 @@
       <c r="K7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
       <c r="N7" s="9"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
@@ -1054,8 +1054,8 @@
       <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
@@ -1071,8 +1071,8 @@
       <c r="K9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
       <c r="N9" s="9"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
@@ -1088,8 +1088,8 @@
       <c r="K10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
       <c r="N10" s="9"/>
     </row>
     <row r="11" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1108,22 +1108,22 @@
       <c r="N11" s="15"/>
     </row>
     <row r="12" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="33" t="str">
+      <c r="B12" s="32" t="str">
         <f>IF(AND(LEN(L4)&gt;0,LEN(L5)&gt;0,LEN(L6)&gt;0,LEN(L7)&gt;0,LEN(L8)&gt;0,LEN(L9)&gt;0,LEN(L10)&gt;0),"Complete","Incomplete")</f>
         <v>Incomplete</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="35"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="34"/>
     </row>
     <row r="13" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17"/>
@@ -1185,8 +1185,8 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="20"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
       <c r="N16" s="9"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
@@ -1200,8 +1200,8 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="20"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
       <c r="N17" s="9"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
@@ -1227,8 +1227,8 @@
       <c r="K18" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
       <c r="N18" s="9"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
@@ -1240,8 +1240,8 @@
       <c r="I19" s="31"/>
       <c r="J19" s="31"/>
       <c r="K19" s="31"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
       <c r="N19" s="9"/>
     </row>
     <row r="20" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1260,22 +1260,22 @@
       <c r="N20" s="15"/>
     </row>
     <row r="21" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="33" t="str">
+      <c r="B21" s="32" t="str">
         <f>IF(AND(LEN(E19)&gt;0,LEN(F19)&gt;0,LEN(G19)&gt;0,LEN(H19)&gt;0,LEN(I19)&gt;0,LEN(J19)&gt;0,LEN(K19)&gt;0),"Complete","Incomplete")</f>
         <v>Incomplete</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="35"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="34"/>
     </row>
     <row r="22" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
@@ -1323,8 +1323,8 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="20"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
       <c r="N25" s="9"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
@@ -1338,8 +1338,8 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="20"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
       <c r="N26" s="9"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
@@ -1350,14 +1350,14 @@
       <c r="F27" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="36" t="s">
+      <c r="G27" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="H27" s="37"/>
-      <c r="I27" s="36" t="s">
+      <c r="H27" s="38"/>
+      <c r="I27" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="J27" s="37"/>
+      <c r="J27" s="38"/>
       <c r="K27" s="20"/>
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
@@ -1371,10 +1371,10 @@
       <c r="F28" s="25">
         <v>1</v>
       </c>
-      <c r="G28" s="38"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="40"/>
       <c r="K28" s="20"/>
       <c r="L28" s="16"/>
       <c r="M28" s="16"/>
@@ -1386,13 +1386,13 @@
       <c r="F29" s="25">
         <v>2</v>
       </c>
-      <c r="G29" s="38"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="40"/>
       <c r="K29" s="22"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
       <c r="N29" s="9"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
@@ -1401,13 +1401,13 @@
       <c r="F30" s="25">
         <v>3</v>
       </c>
-      <c r="G30" s="38"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="40"/>
       <c r="K30" s="24"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
       <c r="N30" s="9"/>
     </row>
     <row r="31" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1426,22 +1426,22 @@
       <c r="N31" s="15"/>
     </row>
     <row r="32" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="33" t="str">
+      <c r="B32" s="32" t="str">
         <f>IF(AND(LEN(G28)&gt;0,LEN(G29)&gt;0,LEN(G30)&gt;0,LEN(I28)&gt;0,LEN(I29)&gt;0,LEN(I30)&gt;0),"Complete","Incomplete")</f>
         <v>Incomplete</v>
       </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="35"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="34"/>
     </row>
     <row r="33" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
@@ -1489,8 +1489,8 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="20"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="35"/>
       <c r="N36" s="9"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
@@ -1504,8 +1504,8 @@
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="20"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
       <c r="N37" s="9"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
@@ -1589,8 +1589,8 @@
       <c r="K40" s="19">
         <v>0</v>
       </c>
-      <c r="L40" s="32"/>
-      <c r="M40" s="32"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
       <c r="N40" s="9"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
@@ -1616,8 +1616,8 @@
       <c r="K41" s="19">
         <v>1</v>
       </c>
-      <c r="L41" s="32"/>
-      <c r="M41" s="32"/>
+      <c r="L41" s="35"/>
+      <c r="M41" s="35"/>
       <c r="N41" s="9"/>
     </row>
     <row r="42" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1636,43 +1636,25 @@
       <c r="N42" s="15"/>
     </row>
     <row r="43" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="33" t="str">
+      <c r="B43" s="32" t="str">
         <f>IF(SUM(E38:K41)=0,"Complete","Incomplete")</f>
         <v>Incomplete</v>
       </c>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
-      <c r="K43" s="34"/>
-      <c r="L43" s="34"/>
-      <c r="M43" s="34"/>
-      <c r="N43" s="35"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B43:N43"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="B21:N21"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="B12:N12"/>
     <mergeCell ref="L25:M25"/>
     <mergeCell ref="L26:M26"/>
     <mergeCell ref="L29:M29"/>
@@ -1686,6 +1668,24 @@
     <mergeCell ref="I28:J28"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="I30:J30"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="B21:N21"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="B12:N12"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="B43:N43"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="L37:M37"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:N13">
     <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="Incomplete">

</xml_diff>

<commit_message>
Add edit mode lesson
</commit_message>
<xml_diff>
--- a/ExcelCo/basics/02_data_entry.xlsx
+++ b/ExcelCo/basics/02_data_entry.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="340" yWindow="700" windowWidth="24960" windowHeight="13840" tabRatio="500"/>
+    <workbookView xWindow="340" yWindow="700" windowWidth="24960" windowHeight="13840" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lessons" sheetId="1" r:id="rId1"/>
@@ -207,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -373,24 +373,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -449,48 +436,49 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -930,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -986,8 +974,8 @@
       <c r="K4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
       <c r="N4" s="9"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
@@ -1003,8 +991,8 @@
       <c r="K5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
       <c r="N5" s="9"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
@@ -1020,8 +1008,8 @@
       <c r="K6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
       <c r="N6" s="9"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
@@ -1037,8 +1025,8 @@
       <c r="K7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
       <c r="N7" s="9"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
@@ -1054,8 +1042,8 @@
       <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
@@ -1071,8 +1059,8 @@
       <c r="K9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
       <c r="N9" s="9"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
@@ -1088,8 +1076,8 @@
       <c r="K10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
       <c r="N10" s="9"/>
     </row>
     <row r="11" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1108,22 +1096,22 @@
       <c r="N11" s="15"/>
     </row>
     <row r="12" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="32" t="str">
+      <c r="B12" s="31" t="str">
         <f>IF(AND(LEN(L4)&gt;0,LEN(L5)&gt;0,LEN(L6)&gt;0,LEN(L7)&gt;0,LEN(L8)&gt;0,LEN(L9)&gt;0,LEN(L10)&gt;0),"Complete","Incomplete")</f>
         <v>Incomplete</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="34"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="33"/>
     </row>
     <row r="13" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17"/>
@@ -1185,8 +1173,8 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="20"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
       <c r="N16" s="9"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
@@ -1200,8 +1188,8 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="20"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
       <c r="N17" s="9"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
@@ -1227,21 +1215,21 @@
       <c r="K18" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
       <c r="N18" s="9"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="10"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
       <c r="N19" s="9"/>
     </row>
     <row r="20" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1260,22 +1248,22 @@
       <c r="N20" s="15"/>
     </row>
     <row r="21" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="32" t="str">
+      <c r="B21" s="31" t="str">
         <f>IF(AND(LEN(E19)&gt;0,LEN(F19)&gt;0,LEN(G19)&gt;0,LEN(H19)&gt;0,LEN(I19)&gt;0,LEN(J19)&gt;0,LEN(K19)&gt;0),"Complete","Incomplete")</f>
         <v>Incomplete</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="34"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="33"/>
     </row>
     <row r="22" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
@@ -1323,8 +1311,8 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="20"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
       <c r="N25" s="9"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
@@ -1338,8 +1326,8 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="20"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
       <c r="N26" s="9"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
@@ -1350,14 +1338,14 @@
       <c r="F27" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="37" t="s">
+      <c r="G27" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="H27" s="38"/>
-      <c r="I27" s="37" t="s">
+      <c r="H27" s="35"/>
+      <c r="I27" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="J27" s="38"/>
+      <c r="J27" s="35"/>
       <c r="K27" s="20"/>
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
@@ -1371,10 +1359,10 @@
       <c r="F28" s="25">
         <v>1</v>
       </c>
-      <c r="G28" s="39"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="40"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="37"/>
       <c r="K28" s="20"/>
       <c r="L28" s="16"/>
       <c r="M28" s="16"/>
@@ -1386,13 +1374,13 @@
       <c r="F29" s="25">
         <v>2</v>
       </c>
-      <c r="G29" s="39"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="40"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="37"/>
       <c r="K29" s="22"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
       <c r="N29" s="9"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
@@ -1401,13 +1389,13 @@
       <c r="F30" s="25">
         <v>3</v>
       </c>
-      <c r="G30" s="39"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="40"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="37"/>
       <c r="K30" s="24"/>
-      <c r="L30" s="35"/>
-      <c r="M30" s="35"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
       <c r="N30" s="9"/>
     </row>
     <row r="31" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1426,22 +1414,22 @@
       <c r="N31" s="15"/>
     </row>
     <row r="32" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="32" t="str">
+      <c r="B32" s="31" t="str">
         <f>IF(AND(LEN(G28)&gt;0,LEN(G29)&gt;0,LEN(G30)&gt;0,LEN(I28)&gt;0,LEN(I29)&gt;0,LEN(I30)&gt;0),"Complete","Incomplete")</f>
         <v>Incomplete</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="34"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="33"/>
     </row>
     <row r="33" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
@@ -1489,8 +1477,8 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="20"/>
-      <c r="L36" s="35"/>
-      <c r="M36" s="35"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="30"/>
       <c r="N36" s="9"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
@@ -1504,8 +1492,8 @@
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="20"/>
-      <c r="L37" s="35"/>
-      <c r="M37" s="35"/>
+      <c r="L37" s="30"/>
+      <c r="M37" s="30"/>
       <c r="N37" s="9"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
@@ -1589,8 +1577,8 @@
       <c r="K40" s="19">
         <v>0</v>
       </c>
-      <c r="L40" s="35"/>
-      <c r="M40" s="35"/>
+      <c r="L40" s="30"/>
+      <c r="M40" s="30"/>
       <c r="N40" s="9"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
@@ -1616,8 +1604,8 @@
       <c r="K41" s="19">
         <v>1</v>
       </c>
-      <c r="L41" s="35"/>
-      <c r="M41" s="35"/>
+      <c r="L41" s="30"/>
+      <c r="M41" s="30"/>
       <c r="N41" s="9"/>
     </row>
     <row r="42" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1636,25 +1624,43 @@
       <c r="N42" s="15"/>
     </row>
     <row r="43" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="32" t="str">
+      <c r="B43" s="31" t="str">
         <f>IF(SUM(E38:K41)=0,"Complete","Incomplete")</f>
         <v>Incomplete</v>
       </c>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="33"/>
-      <c r="L43" s="33"/>
-      <c r="M43" s="33"/>
-      <c r="N43" s="34"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="32"/>
+      <c r="M43" s="32"/>
+      <c r="N43" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B43:N43"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="B21:N21"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="B12:N12"/>
     <mergeCell ref="L25:M25"/>
     <mergeCell ref="L26:M26"/>
     <mergeCell ref="L29:M29"/>
@@ -1668,24 +1674,6 @@
     <mergeCell ref="I28:J28"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="I30:J30"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="B21:N21"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="B12:N12"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="B43:N43"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="L37:M37"/>
   </mergeCells>
   <conditionalFormatting sqref="B12:N13">
     <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="Incomplete">
@@ -1735,9 +1723,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q14"/>
+  <dimension ref="B2:Q15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:Q2"/>
     </sheetView>
   </sheetViews>
@@ -1747,24 +1735,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E4" s="27"/>
@@ -2125,51 +2113,48 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="30" t="str">
+      <c r="F13" s="26" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G13" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H13" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I13" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J13" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="K13" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="L13" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M13" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N13" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="E14" s="42" t="str">
-        <f>IF(SUM(F5:N13)=2025,"Complete","Incomplete")</f>
-        <v>Incomplete</v>
-      </c>
+      <c r="G13" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H13" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I13" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J13" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="K13" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="L13" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M13" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N13" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:17" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="43"/>
       <c r="F14" s="42"/>
       <c r="G14" s="42"/>
       <c r="H14" s="42"/>
@@ -2180,12 +2165,27 @@
       <c r="M14" s="42"/>
       <c r="N14" s="42"/>
     </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="E15" s="40" t="str">
+        <f>IF(SUM(F5:N13)=2025,"Complete","Incomplete")</f>
+        <v>Incomplete</v>
+      </c>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="E14:N14"/>
+    <mergeCell ref="E15:N15"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:N13">
+  <conditionalFormatting sqref="F5:N14">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2197,17 +2197,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:N4 E5:E13">
+  <conditionalFormatting sqref="F4:N4 E5:E14">
     <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(E4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:N14">
+  <conditionalFormatting sqref="E15:N15">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Incomplete">
-      <formula>NOT(ISERROR(SEARCH("Incomplete",E14)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Incomplete",E15)))</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="2" operator="beginsWith" text="Complete">
-      <formula>LEFT(E14,LEN("Complete"))="Complete"</formula>
+      <formula>LEFT(E15,LEN("Complete"))="Complete"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>